<commit_message>
huhu ayo dikit lagi bisa bisa semangat kamu hebattt
</commit_message>
<xml_diff>
--- a/evaluasi/Dokumen Evaluasi Sistem Peringkasan Otomatis.xlsx
+++ b/evaluasi/Dokumen Evaluasi Sistem Peringkasan Otomatis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6600" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6600" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="dok 1" sheetId="2" r:id="rId1"/>
@@ -1493,7 +1493,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1553,6 +1553,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1568,13 +1575,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1870,18 +1871,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -1896,16 +1897,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$46,0)</f>
         <v>2</v>
@@ -1927,28 +1928,28 @@
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -1966,7 +1967,7 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="30"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -1975,7 +1976,7 @@
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="30"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -2000,9 +2001,9 @@
         <v>8</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -2063,7 +2064,7 @@
         <v>85</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="30"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
@@ -2100,8 +2101,8 @@
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
@@ -2109,8 +2110,8 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -2118,8 +2119,8 @@
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
@@ -2127,8 +2128,8 @@
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -2164,7 +2165,7 @@
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="30"/>
+      <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
@@ -2173,7 +2174,7 @@
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="30"/>
+      <c r="E32" s="25"/>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
@@ -2323,18 +2324,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -2349,16 +2350,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$63,0)</f>
         <v>3</v>
@@ -2380,27 +2381,27 @@
       <c r="A5" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="17"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="17"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2408,8 +2409,8 @@
         <v>273</v>
       </c>
       <c r="B8" s="17"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2462,8 +2463,8 @@
         <v>275</v>
       </c>
       <c r="B14" s="17"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="17"/>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -2471,8 +2472,8 @@
         <v>381</v>
       </c>
       <c r="B15" s="17"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="32"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2607,7 +2608,7 @@
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
-      <c r="D30" s="32"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="17"/>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2625,7 +2626,7 @@
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
-      <c r="D32" s="32"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="17"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2643,7 +2644,7 @@
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
-      <c r="D34" s="32"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2661,7 +2662,7 @@
       </c>
       <c r="B36" s="17"/>
       <c r="C36" s="17"/>
-      <c r="D36" s="32"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="17"/>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2670,7 +2671,7 @@
       </c>
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
-      <c r="D37" s="32"/>
+      <c r="D37" s="27"/>
       <c r="E37" s="17"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2715,8 +2716,8 @@
       </c>
       <c r="B42" s="17"/>
       <c r="C42" s="17"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
@@ -2724,8 +2725,8 @@
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="32"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
@@ -2734,7 +2735,7 @@
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
-      <c r="E44" s="32"/>
+      <c r="E44" s="27"/>
     </row>
     <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
@@ -2742,8 +2743,8 @@
       </c>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="32"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="27"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
@@ -2770,7 +2771,7 @@
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
-      <c r="E48" s="34"/>
+      <c r="E48" s="29"/>
     </row>
     <row r="49" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -2779,7 +2780,7 @@
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
-      <c r="E49" s="32"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
@@ -2788,7 +2789,7 @@
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
-      <c r="E50" s="32"/>
+      <c r="E50" s="27"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
@@ -2920,7 +2921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2930,18 +2931,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -2956,16 +2957,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="36"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="16">
         <f>ROUNDUP(0.05*$B$17,0)</f>
         <v>1</v>
@@ -2987,10 +2988,10 @@
       <c r="A5" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
@@ -3007,8 +3008,8 @@
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
@@ -3071,7 +3072,7 @@
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
-      <c r="E14" s="32"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
@@ -3123,18 +3124,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -3149,16 +3150,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$34,0)</f>
         <v>2</v>
@@ -3180,19 +3181,19 @@
       <c r="A5" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -3264,7 +3265,7 @@
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="30"/>
+      <c r="E14" s="25"/>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -3291,7 +3292,7 @@
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="30"/>
+      <c r="E17" s="25"/>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
@@ -3334,9 +3335,9 @@
         <v>61</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -3362,8 +3363,8 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -3380,8 +3381,8 @@
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -3389,7 +3390,7 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="30"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -3408,7 +3409,7 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="30"/>
+      <c r="E30" s="25"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
@@ -3461,18 +3462,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -3487,16 +3488,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$33,0)</f>
         <v>2</v>
@@ -3518,19 +3519,19 @@
       <c r="A5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
@@ -3539,7 +3540,7 @@
       <c r="B7" s="21"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="30"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
@@ -3548,7 +3549,7 @@
       <c r="B8" s="21"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="30"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
@@ -3573,9 +3574,9 @@
         <v>117</v>
       </c>
       <c r="B11" s="21"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
@@ -3593,7 +3594,7 @@
       <c r="B13" s="21"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="30"/>
+      <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
@@ -3727,8 +3728,8 @@
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
@@ -3736,8 +3737,8 @@
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -3745,8 +3746,8 @@
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
@@ -3811,18 +3812,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -3837,16 +3838,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$38,0)</f>
         <v>2</v>
@@ -3868,19 +3869,19 @@
       <c r="A5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -3896,18 +3897,18 @@
         <v>97</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -3924,8 +3925,8 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -4006,7 +4007,7 @@
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
-      <c r="E20" s="30"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
@@ -4069,7 +4070,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="30"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -4086,8 +4087,8 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -4104,8 +4105,8 @@
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
@@ -4141,7 +4142,7 @@
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="30"/>
+      <c r="E35" s="25"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
@@ -4195,18 +4196,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -4221,16 +4222,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="35"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="16">
         <f>ROUNDUP(0.05*$B$61,0)</f>
         <v>3</v>
@@ -4252,46 +4253,46 @@
       <c r="A5" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>126</v>
       </c>
       <c r="B8" s="17"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>127</v>
       </c>
       <c r="B9" s="17"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -4505,9 +4506,9 @@
         <v>140</v>
       </c>
       <c r="B33" s="17"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
     </row>
     <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
@@ -4515,8 +4516,8 @@
       </c>
       <c r="B34" s="17"/>
       <c r="C34" s="17"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
@@ -4551,8 +4552,8 @@
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="17"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
@@ -4578,8 +4579,8 @@
       </c>
       <c r="B41" s="17"/>
       <c r="C41" s="17"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="27"/>
     </row>
     <row r="42" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
@@ -4596,8 +4597,8 @@
       </c>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
-      <c r="D43" s="32"/>
-      <c r="E43" s="32"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
@@ -4641,8 +4642,8 @@
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
@@ -4651,7 +4652,7 @@
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
-      <c r="E49" s="32"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
@@ -4669,7 +4670,7 @@
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
-      <c r="E51" s="32"/>
+      <c r="E51" s="27"/>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
@@ -4687,7 +4688,7 @@
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
-      <c r="E53" s="32"/>
+      <c r="E53" s="27"/>
     </row>
     <row r="54" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
@@ -4696,7 +4697,7 @@
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
-      <c r="E54" s="32"/>
+      <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
@@ -4705,7 +4706,7 @@
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
-      <c r="E55" s="32"/>
+      <c r="E55" s="27"/>
     </row>
     <row r="56" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
@@ -4775,18 +4776,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -4801,16 +4802,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$37,0)</f>
         <v>2</v>
@@ -4832,19 +4833,19 @@
       <c r="A5" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -4869,9 +4870,9 @@
         <v>156</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
@@ -4879,8 +4880,8 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
@@ -4888,8 +4889,8 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -4933,8 +4934,8 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -4961,7 +4962,7 @@
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="30"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
@@ -4979,7 +4980,7 @@
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
-      <c r="E21" s="30"/>
+      <c r="E21" s="25"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
@@ -4988,7 +4989,7 @@
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="30"/>
+      <c r="E22" s="25"/>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -4997,7 +4998,7 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="30"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
@@ -5128,28 +5129,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="73.140625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="3" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -5164,16 +5168,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$40,0)</f>
         <v>2</v>
@@ -5195,10 +5199,10 @@
       <c r="A5" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -5213,10 +5217,10 @@
       <c r="A7" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -5241,18 +5245,18 @@
         <v>186</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>187</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -5287,8 +5291,8 @@
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -5296,8 +5300,8 @@
       </c>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
@@ -5359,8 +5363,8 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
@@ -5369,7 +5373,7 @@
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="30"/>
+      <c r="E24" s="25"/>
     </row>
     <row r="25" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
@@ -5378,7 +5382,7 @@
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="30"/>
+      <c r="E25" s="25"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -5396,7 +5400,7 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="30"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -5509,7 +5513,7 @@
       <c r="A42" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="37" t="s">
         <v>217</v>
       </c>
     </row>
@@ -5519,8 +5523,11 @@
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="A1:A4"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B42" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5538,18 +5545,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -5564,16 +5571,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$39,0)</f>
         <v>2</v>
@@ -5595,8 +5602,8 @@
       <c r="A5" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
     </row>
@@ -5604,8 +5611,8 @@
       <c r="A6" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="32"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
     </row>
@@ -5623,7 +5630,7 @@
         <v>222</v>
       </c>
       <c r="B8" s="23"/>
-      <c r="C8" s="32"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
     </row>
@@ -5632,7 +5639,7 @@
         <v>223</v>
       </c>
       <c r="B9" s="23"/>
-      <c r="C9" s="32"/>
+      <c r="C9" s="27"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
     </row>
@@ -5659,9 +5666,9 @@
         <v>234</v>
       </c>
       <c r="B12" s="23"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
@@ -5697,7 +5704,7 @@
       <c r="B16" s="23"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
-      <c r="E16" s="32"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
@@ -5706,7 +5713,7 @@
       <c r="B17" s="23"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
-      <c r="E17" s="32"/>
+      <c r="E17" s="27"/>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
@@ -5722,18 +5729,18 @@
         <v>227</v>
       </c>
       <c r="B19" s="23"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
     </row>
     <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>228</v>
       </c>
       <c r="B20" s="23"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
@@ -5778,7 +5785,7 @@
       <c r="B25" s="23"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
-      <c r="E25" s="32"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
@@ -5937,18 +5944,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="32"/>
       <c r="B2" s="3">
         <v>0.05</v>
       </c>
@@ -5963,16 +5970,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="32"/>
       <c r="B4" s="4">
         <f>ROUNDUP(0.05*$B$46,0)</f>
         <v>2</v>
@@ -5994,19 +6001,19 @@
       <c r="A5" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -6067,9 +6074,9 @@
         <v>369</v>
       </c>
       <c r="B13" s="17"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
@@ -6193,9 +6200,9 @@
         <v>248</v>
       </c>
       <c r="B27" s="17"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
@@ -6203,8 +6210,8 @@
       </c>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
@@ -6212,8 +6219,8 @@
       </c>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
     </row>
     <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
@@ -6221,8 +6228,8 @@
       </c>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
@@ -6248,8 +6255,8 @@
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
     </row>
     <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
@@ -6267,7 +6274,7 @@
       <c r="B35" s="17"/>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
-      <c r="E35" s="32"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
@@ -6285,7 +6292,7 @@
       <c r="B37" s="17"/>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
-      <c r="E37" s="32"/>
+      <c r="E37" s="27"/>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
@@ -6312,7 +6319,7 @@
       <c r="B40" s="17"/>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
-      <c r="E40" s="32"/>
+      <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
@@ -6339,7 +6346,7 @@
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
-      <c r="E43" s="32"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">

</xml_diff>